<commit_message>
Update Resource Relative Path
</commit_message>
<xml_diff>
--- a/MyFlightParameter/Default.xlsx
+++ b/MyFlightParameter/Default.xlsx
@@ -195,7 +195,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -206,9 +208,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -549,34 +549,34 @@
       </c>
     </row>
     <row>
+      <c s="3" t="s">
+        <v>4</v>
+      </c>
+      <c s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row>
+      <c s="3" t="s">
+        <v>0</v>
+      </c>
       <c s="2" t="s">
         <v>4</v>
       </c>
-      <c s="3" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row>
+      <c s="3" t="s">
+        <v>5</v>
+      </c>
       <c s="2" t="s">
-        <v>0</v>
-      </c>
-      <c s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row>
-      <c s="2" t="s">
-        <v>5</v>
-      </c>
       <c s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row>
       <c s="2" t="s">
-        <v>2</v>
-      </c>
-      <c s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Repo Relative Path
</commit_message>
<xml_diff>
--- a/MyFlightParameter/Default.xlsx
+++ b/MyFlightParameter/Default.xlsx
@@ -195,9 +195,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -208,7 +206,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -549,34 +549,34 @@
       </c>
     </row>
     <row>
+      <c s="2" t="s">
+        <v>4</v>
+      </c>
+      <c s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row>
+      <c s="2" t="s">
+        <v>0</v>
+      </c>
       <c s="3" t="s">
         <v>4</v>
       </c>
-      <c s="2" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row>
+      <c s="2" t="s">
+        <v>5</v>
+      </c>
       <c s="3" t="s">
-        <v>0</v>
-      </c>
-      <c s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row>
-      <c s="3" t="s">
-        <v>5</v>
-      </c>
       <c s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row>
       <c s="3" t="s">
-        <v>2</v>
-      </c>
-      <c s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>